<commit_message>
Ya se lee el excel Portafolio.xlsx
</commit_message>
<xml_diff>
--- a/docs_xlsx/Data.xlsx
+++ b/docs_xlsx/Data.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="erassin 50 mg x 2 tabletas" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="esomeprazol 20 mg x 14 tabletas ag" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="esomeprazol 20 mg x 30 tabletas colmed" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="esomeprazol 40 mg x 30 tabletas colmed" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="etoricoxib 120 mg x 7 tabletas momenta" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -426,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -509,12 +512,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>https://tododrogas.com.co</t>
+          <t>https://www.farmalisto.com.co</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>COP 5,900.00</t>
+          <t>COP 17,385.00</t>
         </is>
       </c>
     </row>
@@ -527,6 +530,18 @@
       <c r="B8" t="inlineStr">
         <is>
           <t xml:space="preserve">COP 18,300.00 </t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>https://tododrogas.com.co</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>COP 5,900.00</t>
         </is>
       </c>
     </row>
@@ -636,4 +651,265 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Link</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>https://www.larebajavirtual.com</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>COP 64,050.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>https://www.farmatodo.com.co</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>COP 42,950.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>https://www.drogueriascolsubsidio.com</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>COP 47,450.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>https://drogueriasfarmavida.com</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>USD 51,900.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>https://www.drogueriascafam.com.co</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>COP 53,900.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>https://www.farmalisto.com.co</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Esomeprazol 20 mg Caja X 30 Tabletas Rx. Ingrediente Activo: ESOMEPRAZOL MAGNESICO TRIHIDRATO22.3MG ( EQUIVALENTE A ESOMEPRAZOL BASE) Reg.</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Link</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>https://www.larebajavirtual.com</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>COP 80,400.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>https://www.farmatodo.com.co</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>COP 54,000.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>https://drogueriasfarmavida.com</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>USD 74,300.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>https://www.drogueriascafam.com.co</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>COP 95,350.00</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Link</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>https://drogueriasfarmavida.com</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>COP 28,839.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>https://www.farmalisto.com.co</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>COP 25,475.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>https://www.cruzverde.com.co</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>COP 42,988.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>https://www.drogueriascafam.com.co</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>COP 45,900.00</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>